<commit_message>
added xor, lui instructions, ran PRPG succuessfully
</commit_message>
<xml_diff>
--- a/Richard/Activity Log.xlsx
+++ b/Richard/Activity Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rremi\Desktop\ECE 366\Hex-Decoder\Richard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A527C3DE-0CA8-4380-AAD8-1668079D96D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08A30DF-64C2-4588-951B-DE44ACE9F0F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Date/Location</t>
   </si>
@@ -111,7 +111,13 @@
     <t>Test the decoder using Project 1 code</t>
   </si>
   <si>
-    <t>Tuesday (2/26/19) 6:00 PM - PM</t>
+    <t>Tuesday (2/26/19) 6:00 PM - 3:00 AM</t>
+  </si>
+  <si>
+    <t>Fixed debugging issues, ran PRPG program successfully</t>
+  </si>
+  <si>
+    <t>Test the decoder using Project 1 code part 2</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,6 +614,15 @@
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added test case 3b, 4b
</commit_message>
<xml_diff>
--- a/Richard/Activity Log.xlsx
+++ b/Richard/Activity Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rremi\Desktop\ECE 366\Hex-Decoder\Richard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08A30DF-64C2-4588-951B-DE44ACE9F0F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2160BAB1-00F5-4933-A8E7-5D38943481AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Date/Location</t>
   </si>
@@ -118,6 +118,30 @@
   </si>
   <si>
     <t>Test the decoder using Project 1 code part 2</t>
+  </si>
+  <si>
+    <t>Wednesday (2/27/19) 6:00 PM - 3:30 AM</t>
+  </si>
+  <si>
+    <t>Fixing sll instruction, get Project 1 hamming weight and distance to work</t>
+  </si>
+  <si>
+    <t>Continue the activity</t>
+  </si>
+  <si>
+    <t>Wednesday (2/27/19) 6:00 PM - 10:30 PM</t>
+  </si>
+  <si>
+    <t>Richard, Syed, Rami</t>
+  </si>
+  <si>
+    <t>Thursday (2/28/19) 6:00 PM - 11:59 PM</t>
+  </si>
+  <si>
+    <t>Finish the project, clean source folders, write lab reports</t>
+  </si>
+  <si>
+    <t>Turn in project</t>
   </si>
 </sst>
 </file>
@@ -483,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CA3FDB-D763-4CE5-9DE9-DF6F5D651576}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,6 +648,48 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>